<commit_message>
Atualizada planilha de resultados
</commit_message>
<xml_diff>
--- a/results/learning_data.xlsx
+++ b/results/learning_data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\segfa\Dev\TCC-Prototype\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B41BD7-9CF6-4375-8BCE-CAECCA291D98}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE312B-52EA-4E54-84E6-900CF989489B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12750" xr2:uid="{D7EAE693-1360-4C4C-A0EA-D45E9444A156}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="12750" xr2:uid="{D7EAE693-1360-4C4C-A0EA-D45E9444A156}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Aprendizado" sheetId="1" r:id="rId1"/>
+    <sheet name="Resultados Sintéticos" sheetId="2" r:id="rId2"/>
+    <sheet name="Resultados Naturais" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Aprendizado</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Erro Treinamento</t>
   </si>
@@ -49,15 +48,48 @@
   <si>
     <t>Época</t>
   </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Parâmetros</t>
+  </si>
+  <si>
+    <t>Resultados</t>
+  </si>
+  <si>
+    <t>Parâmetro</t>
+  </si>
+  <si>
+    <t>Epocas</t>
+  </si>
+  <si>
+    <t>Taxa de Aprendizado</t>
+  </si>
+  <si>
+    <t>Número de  Amostras</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Batch Size</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>2000 por letra</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,13 +124,6 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -126,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -135,10 +160,28 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,7 +299,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$4:$B$67</c:f>
+              <c:f>Aprendizado!$B$14:$B$77</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="64"/>
@@ -482,7 +525,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$4:$C$67</c:f>
+              <c:f>Aprendizado!$C$14:$C$77</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="64"/>
@@ -708,7 +751,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$D$4:$D$67</c:f>
+              <c:f>Aprendizado!$D$14:$D$77</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="64"/>
@@ -934,7 +977,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$E$4:$E$67</c:f>
+              <c:f>Aprendizado!$E$14:$E$77</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="64"/>
@@ -1910,7 +1953,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>200024</xdr:rowOff>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2235,10 +2278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A137F57D-F660-4E71-A9FA-9CC4B1EF2478}">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2250,1118 +2293,1309 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="13">
+        <v>64</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6">
-        <v>3.5996000000000001</v>
-      </c>
-      <c r="C4" s="6">
-        <v>2.9600000000000001E-2</v>
-      </c>
-      <c r="D4" s="6">
-        <v>3.5741999999999998</v>
-      </c>
-      <c r="E4" s="6">
-        <v>4.5400000000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6">
-        <v>3.5745</v>
-      </c>
-      <c r="C5" s="6">
-        <v>3.7400000000000003E-2</v>
-      </c>
-      <c r="D5" s="6">
-        <v>3.5600999999999998</v>
-      </c>
-      <c r="E5" s="6">
-        <v>8.0699999999999994E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6">
-        <v>3.5537999999999998</v>
-      </c>
-      <c r="C6" s="6">
-        <v>4.7600000000000003E-2</v>
-      </c>
-      <c r="D6" s="6">
-        <v>3.5423</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.1008</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6">
-        <v>3.5295999999999998</v>
-      </c>
-      <c r="C7" s="6">
-        <v>5.9700000000000003E-2</v>
-      </c>
-      <c r="D7" s="6">
-        <v>3.5124</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0.1295</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>5</v>
-      </c>
-      <c r="B8" s="6">
-        <v>3.4851000000000001</v>
-      </c>
-      <c r="C8" s="6">
-        <v>7.4700000000000003E-2</v>
-      </c>
-      <c r="D8" s="6">
-        <v>3.4542999999999999</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.1653</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6">
-        <v>3.4018999999999999</v>
-      </c>
-      <c r="C9" s="6">
-        <v>9.9599999999999994E-2</v>
-      </c>
-      <c r="D9" s="6">
-        <v>3.3275999999999999</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0.24510000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6">
-        <v>3.2421000000000002</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.13880000000000001</v>
-      </c>
-      <c r="D10" s="6">
-        <v>3.0682999999999998</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0.3523</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>8</v>
-      </c>
-      <c r="B11" s="6">
-        <v>2.9912000000000001</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0.1961</v>
-      </c>
-      <c r="D11" s="6">
-        <v>2.7113999999999998</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0.4461</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6">
-        <v>2.7538999999999998</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0.25440000000000002</v>
-      </c>
-      <c r="D12" s="6">
-        <v>2.4243999999999999</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0.50590000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>10</v>
-      </c>
-      <c r="B13" s="6">
-        <v>2.5385</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0.307</v>
-      </c>
-      <c r="D13" s="6">
-        <v>2.1958000000000002</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0.54469999999999996</v>
-      </c>
-    </row>
+    </row>
+    <row r="13" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B14" s="6">
-        <v>2.3679999999999999</v>
+        <v>3.5996000000000001</v>
       </c>
       <c r="C14" s="6">
-        <v>0.35449999999999998</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="D14" s="6">
-        <v>2.0167999999999999</v>
+        <v>3.5741999999999998</v>
       </c>
       <c r="E14" s="6">
-        <v>0.57899999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4.5400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B15" s="6">
-        <v>2.2071999999999998</v>
+        <v>3.5745</v>
       </c>
       <c r="C15" s="6">
-        <v>0.3972</v>
+        <v>3.7400000000000003E-2</v>
       </c>
       <c r="D15" s="6">
-        <v>1.8552</v>
+        <v>3.5600999999999998</v>
       </c>
       <c r="E15" s="6">
-        <v>0.60029999999999994</v>
+        <v>8.0699999999999994E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B16" s="6">
-        <v>2.0718999999999999</v>
+        <v>3.5537999999999998</v>
       </c>
       <c r="C16" s="6">
-        <v>0.4365</v>
+        <v>4.7600000000000003E-2</v>
       </c>
       <c r="D16" s="6">
-        <v>1.7253000000000001</v>
+        <v>3.5423</v>
       </c>
       <c r="E16" s="6">
-        <v>0.62739999999999996</v>
+        <v>0.1008</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B17" s="6">
-        <v>1.9594</v>
+        <v>3.5295999999999998</v>
       </c>
       <c r="C17" s="6">
-        <v>0.4698</v>
+        <v>5.9700000000000003E-2</v>
       </c>
       <c r="D17" s="6">
-        <v>1.6067</v>
+        <v>3.5124</v>
       </c>
       <c r="E17" s="6">
-        <v>0.65369999999999995</v>
+        <v>0.1295</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B18" s="6">
-        <v>1.8555999999999999</v>
+        <v>3.4851000000000001</v>
       </c>
       <c r="C18" s="6">
-        <v>0.50119999999999998</v>
+        <v>7.4700000000000003E-2</v>
       </c>
       <c r="D18" s="6">
-        <v>1.5226</v>
+        <v>3.4542999999999999</v>
       </c>
       <c r="E18" s="6">
-        <v>0.66830000000000001</v>
+        <v>0.1653</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B19" s="6">
-        <v>1.7594000000000001</v>
+        <v>3.4018999999999999</v>
       </c>
       <c r="C19" s="6">
-        <v>0.52839999999999998</v>
+        <v>9.9599999999999994E-2</v>
       </c>
       <c r="D19" s="6">
-        <v>1.4378</v>
+        <v>3.3275999999999999</v>
       </c>
       <c r="E19" s="6">
-        <v>0.68459999999999999</v>
+        <v>0.24510000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B20" s="6">
-        <v>1.6927000000000001</v>
+        <v>3.2421000000000002</v>
       </c>
       <c r="C20" s="6">
-        <v>0.54930000000000001</v>
+        <v>0.13880000000000001</v>
       </c>
       <c r="D20" s="6">
-        <v>1.379</v>
+        <v>3.0682999999999998</v>
       </c>
       <c r="E20" s="6">
-        <v>0.69579999999999997</v>
+        <v>0.3523</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B21" s="6">
-        <v>1.6205000000000001</v>
+        <v>2.9912000000000001</v>
       </c>
       <c r="C21" s="6">
-        <v>0.5696</v>
+        <v>0.1961</v>
       </c>
       <c r="D21" s="6">
-        <v>1.3137000000000001</v>
+        <v>2.7113999999999998</v>
       </c>
       <c r="E21" s="6">
-        <v>0.70450000000000002</v>
+        <v>0.4461</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B22" s="6">
-        <v>1.5595000000000001</v>
+        <v>2.7538999999999998</v>
       </c>
       <c r="C22" s="6">
-        <v>0.58620000000000005</v>
+        <v>0.25440000000000002</v>
       </c>
       <c r="D22" s="6">
-        <v>1.2629999999999999</v>
+        <v>2.4243999999999999</v>
       </c>
       <c r="E22" s="6">
-        <v>0.72109999999999996</v>
+        <v>0.50590000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B23" s="6">
-        <v>1.5052000000000001</v>
+        <v>2.5385</v>
       </c>
       <c r="C23" s="6">
-        <v>0.60389999999999999</v>
+        <v>0.307</v>
       </c>
       <c r="D23" s="6">
-        <v>1.2238</v>
+        <v>2.1958000000000002</v>
       </c>
       <c r="E23" s="6">
-        <v>0.73340000000000005</v>
+        <v>0.54469999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B24" s="6">
-        <v>1.4631000000000001</v>
+        <v>2.3679999999999999</v>
       </c>
       <c r="C24" s="6">
-        <v>0.61680000000000001</v>
+        <v>0.35449999999999998</v>
       </c>
       <c r="D24" s="6">
-        <v>1.1826000000000001</v>
+        <v>2.0167999999999999</v>
       </c>
       <c r="E24" s="6">
-        <v>0.73970000000000002</v>
+        <v>0.57899999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B25" s="6">
-        <v>1.4240999999999999</v>
+        <v>2.2071999999999998</v>
       </c>
       <c r="C25" s="6">
-        <v>0.62670000000000003</v>
+        <v>0.3972</v>
       </c>
       <c r="D25" s="6">
-        <v>1.1487000000000001</v>
+        <v>1.8552</v>
       </c>
       <c r="E25" s="6">
-        <v>0.74729999999999996</v>
+        <v>0.60029999999999994</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B26" s="6">
-        <v>1.3763000000000001</v>
+        <v>2.0718999999999999</v>
       </c>
       <c r="C26" s="6">
-        <v>0.64129999999999998</v>
+        <v>0.4365</v>
       </c>
       <c r="D26" s="6">
-        <v>1.1116999999999999</v>
+        <v>1.7253000000000001</v>
       </c>
       <c r="E26" s="6">
-        <v>0.76119999999999999</v>
+        <v>0.62739999999999996</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B27" s="6">
-        <v>1.3435999999999999</v>
+        <v>1.9594</v>
       </c>
       <c r="C27" s="6">
-        <v>0.6532</v>
+        <v>0.4698</v>
       </c>
       <c r="D27" s="6">
-        <v>1.0865</v>
+        <v>1.6067</v>
       </c>
       <c r="E27" s="6">
-        <v>0.76529999999999998</v>
+        <v>0.65369999999999995</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B28" s="6">
-        <v>1.3124</v>
+        <v>1.8555999999999999</v>
       </c>
       <c r="C28" s="6">
-        <v>0.66180000000000005</v>
+        <v>0.50119999999999998</v>
       </c>
       <c r="D28" s="6">
-        <v>1.0649</v>
+        <v>1.5226</v>
       </c>
       <c r="E28" s="6">
-        <v>0.77339999999999998</v>
+        <v>0.66830000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B29" s="6">
-        <v>1.2870999999999999</v>
+        <v>1.7594000000000001</v>
       </c>
       <c r="C29" s="6">
-        <v>0.66959999999999997</v>
+        <v>0.52839999999999998</v>
       </c>
       <c r="D29" s="6">
-        <v>1.0369999999999999</v>
+        <v>1.4378</v>
       </c>
       <c r="E29" s="6">
-        <v>0.77690000000000003</v>
+        <v>0.68459999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B30" s="6">
-        <v>1.2625</v>
+        <v>1.6927000000000001</v>
       </c>
       <c r="C30" s="6">
-        <v>0.6754</v>
+        <v>0.54930000000000001</v>
       </c>
       <c r="D30" s="6">
-        <v>1.0213000000000001</v>
+        <v>1.379</v>
       </c>
       <c r="E30" s="6">
-        <v>0.78320000000000001</v>
+        <v>0.69579999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B31" s="6">
-        <v>1.2370000000000001</v>
+        <v>1.6205000000000001</v>
       </c>
       <c r="C31" s="6">
-        <v>0.68120000000000003</v>
+        <v>0.5696</v>
       </c>
       <c r="D31" s="6">
-        <v>1.0036</v>
+        <v>1.3137000000000001</v>
       </c>
       <c r="E31" s="6">
-        <v>0.78349999999999997</v>
+        <v>0.70450000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
+        <v>19</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1.5595000000000001</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.58620000000000005</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1.2629999999999999</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.72109999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>20</v>
+      </c>
+      <c r="B33" s="6">
+        <v>1.5052000000000001</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.60389999999999999</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1.2238</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.73340000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>21</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1.4631000000000001</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0.61680000000000001</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1.1826000000000001</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.73970000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>22</v>
+      </c>
+      <c r="B35" s="6">
+        <v>1.4240999999999999</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.62670000000000003</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1.1487000000000001</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.74729999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>23</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1.3763000000000001</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.64129999999999998</v>
+      </c>
+      <c r="D36" s="6">
+        <v>1.1116999999999999</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.76119999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>24</v>
+      </c>
+      <c r="B37" s="6">
+        <v>1.3435999999999999</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0.6532</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1.0865</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.76529999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>25</v>
+      </c>
+      <c r="B38" s="6">
+        <v>1.3124</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.66180000000000005</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1.0649</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.77339999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>26</v>
+      </c>
+      <c r="B39" s="6">
+        <v>1.2870999999999999</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.66959999999999997</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1.0369999999999999</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0.77690000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>27</v>
+      </c>
+      <c r="B40" s="6">
+        <v>1.2625</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0.6754</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1.0213000000000001</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0.78320000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>28</v>
+      </c>
+      <c r="B41" s="6">
+        <v>1.2370000000000001</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0.68120000000000003</v>
+      </c>
+      <c r="D41" s="6">
+        <v>1.0036</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0.78349999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
         <v>29</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B42" s="6">
         <v>1.2098</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C42" s="6">
         <v>0.69279999999999997</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D42" s="6">
         <v>0.97909999999999997</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E42" s="6">
         <v>0.79020000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
         <v>30</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B43" s="6">
         <v>1.1962999999999999</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C43" s="6">
         <v>0.69820000000000004</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D43" s="6">
         <v>0.96830000000000005</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E43" s="6">
         <v>0.79320000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
         <v>31</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B44" s="6">
         <v>1.1657999999999999</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C44" s="6">
         <v>0.70540000000000003</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D44" s="6">
         <v>0.95069999999999999</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E44" s="6">
         <v>0.7994</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
         <v>32</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B45" s="6">
         <v>1.1519999999999999</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C45" s="6">
         <v>0.71130000000000004</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D45" s="6">
         <v>0.93910000000000005</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E45" s="6">
         <v>0.80210000000000004</v>
       </c>
-      <c r="K35" s="7"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
         <v>33</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B46" s="6">
         <v>1.1368</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C46" s="6">
         <v>0.71189999999999998</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D46" s="6">
         <v>0.92530000000000001</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E46" s="6">
         <v>0.80579999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
         <v>34</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B47" s="6">
         <v>1.1202000000000001</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C47" s="6">
         <v>0.72</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D47" s="6">
         <v>0.91220000000000001</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E47" s="6">
         <v>0.80620000000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
         <v>35</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B48" s="6">
         <v>1.1107</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C48" s="6">
         <v>0.72289999999999999</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D48" s="6">
         <v>0.90169999999999995</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E48" s="6">
         <v>0.81040000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
-        <v>36</v>
-      </c>
-      <c r="B39" s="6">
-        <v>1.0924</v>
-      </c>
-      <c r="C39" s="6">
-        <v>0.72729999999999995</v>
-      </c>
-      <c r="D39" s="6">
-        <v>0.8931</v>
-      </c>
-      <c r="E39" s="6">
-        <v>0.8125</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
-        <v>37</v>
-      </c>
-      <c r="B40" s="6">
-        <v>1.0822000000000001</v>
-      </c>
-      <c r="C40" s="6">
-        <v>0.73019999999999996</v>
-      </c>
-      <c r="D40" s="6">
-        <v>0.88139999999999996</v>
-      </c>
-      <c r="E40" s="6">
-        <v>0.81469999999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
-        <v>38</v>
-      </c>
-      <c r="B41" s="6">
-        <v>1.0671999999999999</v>
-      </c>
-      <c r="C41" s="6">
-        <v>0.73309999999999997</v>
-      </c>
-      <c r="D41" s="6">
-        <v>0.87360000000000004</v>
-      </c>
-      <c r="E41" s="6">
-        <v>0.81440000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
-        <v>39</v>
-      </c>
-      <c r="B42" s="6">
-        <v>1.0593999999999999</v>
-      </c>
-      <c r="C42" s="6">
-        <v>0.73860000000000003</v>
-      </c>
-      <c r="D42" s="6">
-        <v>0.86709999999999998</v>
-      </c>
-      <c r="E42" s="6">
-        <v>0.8165</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
-        <v>40</v>
-      </c>
-      <c r="B43" s="6">
-        <v>1.0513999999999999</v>
-      </c>
-      <c r="C43" s="6">
-        <v>0.74080000000000001</v>
-      </c>
-      <c r="D43" s="6">
-        <v>0.85680000000000001</v>
-      </c>
-      <c r="E43" s="6">
-        <v>0.81840000000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
-        <v>41</v>
-      </c>
-      <c r="B44" s="6">
-        <v>1.0387</v>
-      </c>
-      <c r="C44" s="6">
-        <v>0.74180000000000001</v>
-      </c>
-      <c r="D44" s="6">
-        <v>0.84899999999999998</v>
-      </c>
-      <c r="E44" s="6">
-        <v>0.82110000000000005</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
-        <v>42</v>
-      </c>
-      <c r="B45" s="6">
-        <v>1.024</v>
-      </c>
-      <c r="C45" s="6">
-        <v>0.74839999999999995</v>
-      </c>
-      <c r="D45" s="6">
-        <v>0.84460000000000002</v>
-      </c>
-      <c r="E45" s="6">
-        <v>0.82050000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
-        <v>43</v>
-      </c>
-      <c r="B46" s="6">
-        <v>1.0097</v>
-      </c>
-      <c r="C46" s="6">
-        <v>0.75249999999999995</v>
-      </c>
-      <c r="D46" s="6">
-        <v>0.83440000000000003</v>
-      </c>
-      <c r="E46" s="6">
-        <v>0.82289999999999996</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
-        <v>44</v>
-      </c>
-      <c r="B47" s="6">
-        <v>1.004</v>
-      </c>
-      <c r="C47" s="6">
-        <v>0.75390000000000001</v>
-      </c>
-      <c r="D47" s="6">
-        <v>0.8296</v>
-      </c>
-      <c r="E47" s="6">
-        <v>0.82279999999999998</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
-        <v>45</v>
-      </c>
-      <c r="B48" s="6">
-        <v>1.0007999999999999</v>
-      </c>
-      <c r="C48" s="6">
-        <v>0.75490000000000002</v>
-      </c>
-      <c r="D48" s="6">
-        <v>0.82320000000000004</v>
-      </c>
-      <c r="E48" s="6">
-        <v>0.82469999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B49" s="6">
-        <v>0.98740000000000006</v>
+        <v>1.0924</v>
       </c>
       <c r="C49" s="6">
-        <v>0.75929999999999997</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="D49" s="6">
-        <v>0.81830000000000003</v>
+        <v>0.8931</v>
       </c>
       <c r="E49" s="6">
-        <v>0.82689999999999997</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B50" s="6">
-        <v>0.98140000000000005</v>
+        <v>1.0822000000000001</v>
       </c>
       <c r="C50" s="6">
-        <v>0.76039999999999996</v>
+        <v>0.73019999999999996</v>
       </c>
       <c r="D50" s="6">
-        <v>0.80869999999999997</v>
+        <v>0.88139999999999996</v>
       </c>
       <c r="E50" s="6">
-        <v>0.82709999999999995</v>
+        <v>0.81469999999999998</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B51" s="6">
-        <v>0.97260000000000002</v>
+        <v>1.0671999999999999</v>
       </c>
       <c r="C51" s="6">
-        <v>0.76359999999999995</v>
+        <v>0.73309999999999997</v>
       </c>
       <c r="D51" s="6">
-        <v>0.80620000000000003</v>
+        <v>0.87360000000000004</v>
       </c>
       <c r="E51" s="6">
-        <v>0.82909999999999995</v>
+        <v>0.81440000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B52" s="6">
-        <v>0.96630000000000005</v>
+        <v>1.0593999999999999</v>
       </c>
       <c r="C52" s="6">
-        <v>0.76570000000000005</v>
+        <v>0.73860000000000003</v>
       </c>
       <c r="D52" s="6">
-        <v>0.79879999999999995</v>
+        <v>0.86709999999999998</v>
       </c>
       <c r="E52" s="6">
-        <v>0.82940000000000003</v>
+        <v>0.8165</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B53" s="6">
-        <v>0.95689999999999997</v>
+        <v>1.0513999999999999</v>
       </c>
       <c r="C53" s="6">
-        <v>0.76870000000000005</v>
+        <v>0.74080000000000001</v>
       </c>
       <c r="D53" s="6">
-        <v>0.79500000000000004</v>
+        <v>0.85680000000000001</v>
       </c>
       <c r="E53" s="6">
-        <v>0.83089999999999997</v>
+        <v>0.81840000000000002</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B54" s="6">
-        <v>0.95140000000000002</v>
+        <v>1.0387</v>
       </c>
       <c r="C54" s="6">
-        <v>0.76890000000000003</v>
+        <v>0.74180000000000001</v>
       </c>
       <c r="D54" s="6">
-        <v>0.78990000000000005</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="E54" s="6">
-        <v>0.83230000000000004</v>
+        <v>0.82110000000000005</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B55" s="6">
-        <v>0.94610000000000005</v>
+        <v>1.024</v>
       </c>
       <c r="C55" s="6">
-        <v>0.77270000000000005</v>
+        <v>0.74839999999999995</v>
       </c>
       <c r="D55" s="6">
-        <v>0.7853</v>
+        <v>0.84460000000000002</v>
       </c>
       <c r="E55" s="6">
-        <v>0.83320000000000005</v>
+        <v>0.82050000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B56" s="6">
-        <v>0.93840000000000001</v>
+        <v>1.0097</v>
       </c>
       <c r="C56" s="6">
-        <v>0.77410000000000001</v>
+        <v>0.75249999999999995</v>
       </c>
       <c r="D56" s="6">
-        <v>0.77910000000000001</v>
+        <v>0.83440000000000003</v>
       </c>
       <c r="E56" s="6">
-        <v>0.83409999999999995</v>
+        <v>0.82289999999999996</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B57" s="6">
-        <v>0.93789999999999996</v>
+        <v>1.004</v>
       </c>
       <c r="C57" s="6">
-        <v>0.7732</v>
+        <v>0.75390000000000001</v>
       </c>
       <c r="D57" s="6">
-        <v>0.77729999999999999</v>
+        <v>0.8296</v>
       </c>
       <c r="E57" s="6">
-        <v>0.83399999999999996</v>
+        <v>0.82279999999999998</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B58" s="6">
-        <v>0.92379999999999995</v>
+        <v>1.0007999999999999</v>
       </c>
       <c r="C58" s="6">
-        <v>0.77729999999999999</v>
+        <v>0.75490000000000002</v>
       </c>
       <c r="D58" s="6">
-        <v>0.77329999999999999</v>
+        <v>0.82320000000000004</v>
       </c>
       <c r="E58" s="6">
-        <v>0.83620000000000005</v>
+        <v>0.82469999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B59" s="6">
-        <v>0.91610000000000003</v>
+        <v>0.98740000000000006</v>
       </c>
       <c r="C59" s="6">
-        <v>0.77769999999999995</v>
+        <v>0.75929999999999997</v>
       </c>
       <c r="D59" s="6">
-        <v>0.76900000000000002</v>
+        <v>0.81830000000000003</v>
       </c>
       <c r="E59" s="6">
-        <v>0.83599999999999997</v>
+        <v>0.82689999999999997</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B60" s="6">
-        <v>0.91569999999999996</v>
+        <v>0.98140000000000005</v>
       </c>
       <c r="C60" s="6">
-        <v>0.78059999999999996</v>
+        <v>0.76039999999999996</v>
       </c>
       <c r="D60" s="6">
-        <v>0.76539999999999997</v>
+        <v>0.80869999999999997</v>
       </c>
       <c r="E60" s="6">
-        <v>0.83560000000000001</v>
+        <v>0.82709999999999995</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B61" s="6">
-        <v>0.90949999999999998</v>
+        <v>0.97260000000000002</v>
       </c>
       <c r="C61" s="6">
-        <v>0.78090000000000004</v>
+        <v>0.76359999999999995</v>
       </c>
       <c r="D61" s="6">
-        <v>0.76149999999999995</v>
+        <v>0.80620000000000003</v>
       </c>
       <c r="E61" s="6">
-        <v>0.83720000000000006</v>
+        <v>0.82909999999999995</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B62" s="6">
-        <v>0.90629999999999999</v>
+        <v>0.96630000000000005</v>
       </c>
       <c r="C62" s="6">
-        <v>0.7823</v>
+        <v>0.76570000000000005</v>
       </c>
       <c r="D62" s="6">
-        <v>0.7571</v>
+        <v>0.79879999999999995</v>
       </c>
       <c r="E62" s="6">
-        <v>0.83779999999999999</v>
+        <v>0.82940000000000003</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B63" s="6">
-        <v>0.8982</v>
+        <v>0.95689999999999997</v>
       </c>
       <c r="C63" s="6">
-        <v>0.78490000000000004</v>
+        <v>0.76870000000000005</v>
       </c>
       <c r="D63" s="6">
-        <v>0.75349999999999995</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="E63" s="6">
-        <v>0.83830000000000005</v>
+        <v>0.83089999999999997</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B64" s="6">
-        <v>0.89600000000000002</v>
+        <v>0.95140000000000002</v>
       </c>
       <c r="C64" s="6">
-        <v>0.7823</v>
+        <v>0.76890000000000003</v>
       </c>
       <c r="D64" s="6">
-        <v>0.75039999999999996</v>
+        <v>0.78990000000000005</v>
       </c>
       <c r="E64" s="6">
-        <v>0.8387</v>
+        <v>0.83230000000000004</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B65" s="6">
-        <v>0.89359999999999995</v>
+        <v>0.94610000000000005</v>
       </c>
       <c r="C65" s="6">
-        <v>0.78490000000000004</v>
+        <v>0.77270000000000005</v>
       </c>
       <c r="D65" s="6">
-        <v>0.74570000000000003</v>
+        <v>0.7853</v>
       </c>
       <c r="E65" s="6">
-        <v>0.83860000000000001</v>
+        <v>0.83320000000000005</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B66" s="6">
-        <v>0.88280000000000003</v>
+        <v>0.93840000000000001</v>
       </c>
       <c r="C66" s="6">
-        <v>0.78820000000000001</v>
+        <v>0.77410000000000001</v>
       </c>
       <c r="D66" s="6">
-        <v>0.74239999999999995</v>
+        <v>0.77910000000000001</v>
       </c>
       <c r="E66" s="6">
-        <v>0.83960000000000001</v>
+        <v>0.83409999999999995</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
+        <v>54</v>
+      </c>
+      <c r="B67" s="6">
+        <v>0.93789999999999996</v>
+      </c>
+      <c r="C67" s="6">
+        <v>0.7732</v>
+      </c>
+      <c r="D67" s="6">
+        <v>0.77729999999999999</v>
+      </c>
+      <c r="E67" s="6">
+        <v>0.83399999999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="4">
+        <v>55</v>
+      </c>
+      <c r="B68" s="6">
+        <v>0.92379999999999995</v>
+      </c>
+      <c r="C68" s="6">
+        <v>0.77729999999999999</v>
+      </c>
+      <c r="D68" s="6">
+        <v>0.77329999999999999</v>
+      </c>
+      <c r="E68" s="6">
+        <v>0.83620000000000005</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="4">
+        <v>56</v>
+      </c>
+      <c r="B69" s="6">
+        <v>0.91610000000000003</v>
+      </c>
+      <c r="C69" s="6">
+        <v>0.77769999999999995</v>
+      </c>
+      <c r="D69" s="6">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="E69" s="6">
+        <v>0.83599999999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="4">
+        <v>57</v>
+      </c>
+      <c r="B70" s="6">
+        <v>0.91569999999999996</v>
+      </c>
+      <c r="C70" s="6">
+        <v>0.78059999999999996</v>
+      </c>
+      <c r="D70" s="6">
+        <v>0.76539999999999997</v>
+      </c>
+      <c r="E70" s="6">
+        <v>0.83560000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="4">
+        <v>58</v>
+      </c>
+      <c r="B71" s="6">
+        <v>0.90949999999999998</v>
+      </c>
+      <c r="C71" s="6">
+        <v>0.78090000000000004</v>
+      </c>
+      <c r="D71" s="6">
+        <v>0.76149999999999995</v>
+      </c>
+      <c r="E71" s="6">
+        <v>0.83720000000000006</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="4">
+        <v>59</v>
+      </c>
+      <c r="B72" s="6">
+        <v>0.90629999999999999</v>
+      </c>
+      <c r="C72" s="6">
+        <v>0.7823</v>
+      </c>
+      <c r="D72" s="6">
+        <v>0.7571</v>
+      </c>
+      <c r="E72" s="6">
+        <v>0.83779999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
+        <v>60</v>
+      </c>
+      <c r="B73" s="6">
+        <v>0.8982</v>
+      </c>
+      <c r="C73" s="6">
+        <v>0.78490000000000004</v>
+      </c>
+      <c r="D73" s="6">
+        <v>0.75349999999999995</v>
+      </c>
+      <c r="E73" s="6">
+        <v>0.83830000000000005</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="4">
+        <v>61</v>
+      </c>
+      <c r="B74" s="6">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="C74" s="6">
+        <v>0.7823</v>
+      </c>
+      <c r="D74" s="6">
+        <v>0.75039999999999996</v>
+      </c>
+      <c r="E74" s="6">
+        <v>0.8387</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="4">
+        <v>62</v>
+      </c>
+      <c r="B75" s="6">
+        <v>0.89359999999999995</v>
+      </c>
+      <c r="C75" s="6">
+        <v>0.78490000000000004</v>
+      </c>
+      <c r="D75" s="6">
+        <v>0.74570000000000003</v>
+      </c>
+      <c r="E75" s="6">
+        <v>0.83860000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="4">
+        <v>63</v>
+      </c>
+      <c r="B76" s="6">
+        <v>0.88280000000000003</v>
+      </c>
+      <c r="C76" s="6">
+        <v>0.78820000000000001</v>
+      </c>
+      <c r="D76" s="6">
+        <v>0.74239999999999995</v>
+      </c>
+      <c r="E76" s="6">
+        <v>0.83960000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="4">
         <v>64</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B77" s="6">
         <v>0.87939999999999996</v>
       </c>
-      <c r="C67" s="6">
+      <c r="C77" s="6">
         <v>0.79090000000000005</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D77" s="6">
         <v>0.74160000000000004</v>
       </c>
-      <c r="E67" s="6">
+      <c r="E77" s="6">
         <v>0.84060000000000001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B5130274-26AA-48D7-9117-95DD75A3AC15}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Aprendizado!A14:A77</xm:f>
+              <xm:sqref>A13</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D694E7FF-FE18-4A66-8D86-ECE08902F17C}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Aprendizado!E14:E77</xm:f>
+              <xm:sqref>E13</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{F22AFD28-072D-4E54-AB22-1E5958211E31}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Aprendizado!D14:D77</xm:f>
+              <xm:sqref>D13</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{351459D4-AB1F-4275-BF62-D9316746F3B5}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Aprendizado!C14:C77</xm:f>
+              <xm:sqref>C13</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D8735852-2FEC-4BA7-B3D8-4183F761CDB4}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Aprendizado!B14:B77</xm:f>
+              <xm:sqref>B13</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF4F291-2523-4085-82BF-6147FC21D9B0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDA32F7-F326-4E4D-A2B9-D5605DCC9E15}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>